<commit_message>
Moved Calvin nodes around.
</commit_message>
<xml_diff>
--- a/Workflow/dahl nodes.xlsx
+++ b/Workflow/dahl nodes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="38">
   <si>
     <t>Node</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>R version 2.1</t>
+  </si>
+  <si>
+    <t>US, UK, JP</t>
+  </si>
+  <si>
+    <t>CN, ZA, SA</t>
+  </si>
+  <si>
+    <t>IR, TZ, ZM</t>
+  </si>
+  <si>
+    <t>US, UK, JP, CN, ZA, SA, IR, TZ, ZM</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -192,7 +204,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -354,14 +366,154 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,8 +526,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="301">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -456,6 +611,76 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -536,6 +761,76 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1686,9 +1981,9 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1460" topLeftCell="A8" activePane="bottomLeft"/>
-      <selection activeCell="I4" sqref="I4"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="1460" topLeftCell="A20" activePane="bottomLeft"/>
+      <selection activeCell="L3" sqref="L3"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1698,7 +1993,9 @@
     <col min="5" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="2.6640625" style="1" customWidth="1"/>
-    <col min="8" max="14" width="10.83203125" style="1"/>
+    <col min="8" max="11" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="3" style="1" customWidth="1"/>
+    <col min="13" max="15" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1721,12 +2018,16 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
-      <c r="P3" t="s">
+      <c r="L3" s="5"/>
+      <c r="N3" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -1756,10 +2057,19 @@
       <c r="K4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="M4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1767,24 +2077,39 @@
       <c r="A5">
         <v>1</v>
       </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6">
         <v>2</v>
       </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
         <v>3</v>
       </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
         <v>4</v>
       </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="M9">
         <v>5</v>
       </c>
     </row>
@@ -1805,11 +2130,19 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="2">
+        <v>6</v>
+      </c>
       <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17">
       <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="M11">
         <v>7</v>
       </c>
     </row>
@@ -1830,8 +2163,13 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="2">
+        <v>8</v>
+      </c>
       <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13">
@@ -1848,6 +2186,9 @@
       </c>
       <c r="F13" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1872,8 +2213,9 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="M14">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:17" s="2" customFormat="1">
       <c r="A15" s="2">
@@ -1892,8 +2234,13 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="M15" s="2">
+        <v>11</v>
+      </c>
       <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16">
@@ -1911,8 +2258,12 @@
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="M16">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1928,8 +2279,11 @@
       <c r="F17" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="M17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1945,8 +2299,23 @@
       <c r="F18" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="M18">
+        <v>14</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1962,8 +2331,23 @@
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="M19">
+        <v>15</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1979,8 +2363,23 @@
       <c r="F20" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="M20">
+        <v>16</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1996,8 +2395,23 @@
       <c r="F21" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="M21">
+        <v>17</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2013,8 +2427,23 @@
       <c r="F22" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="M22">
+        <v>18</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2030,8 +2459,23 @@
       <c r="F23" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="M23">
+        <v>19</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2047,8 +2491,23 @@
       <c r="F24" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="M24">
+        <v>20</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2076,8 +2535,23 @@
       <c r="K25" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="M25">
+        <v>21</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2105,8 +2579,23 @@
       <c r="K26" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="M26">
+        <v>22</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2134,8 +2623,23 @@
       <c r="K27" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" s="2" customFormat="1">
+      <c r="M27">
+        <v>23</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" s="2" customFormat="1">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -2152,10 +2656,15 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="2">
+        <v>24</v>
+      </c>
       <c r="N28" s="4"/>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2183,8 +2692,23 @@
       <c r="K29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="M29">
+        <v>25</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2212,8 +2736,23 @@
       <c r="K30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" s="2" customFormat="1">
+      <c r="M30">
+        <v>26</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="2" customFormat="1">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -2230,10 +2769,15 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="M31" s="2">
+        <v>27</v>
+      </c>
       <c r="N31" s="4"/>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>28</v>
       </c>
@@ -2261,8 +2805,23 @@
       <c r="K32" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="M32">
+        <v>28</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>29</v>
       </c>
@@ -2290,8 +2849,23 @@
       <c r="K33" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="M33">
+        <v>29</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>30</v>
       </c>
@@ -2319,8 +2893,23 @@
       <c r="K34" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" s="2" customFormat="1">
+      <c r="M34">
+        <v>30</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" s="2" customFormat="1">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -2337,10 +2926,15 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="M35" s="2">
+        <v>31</v>
+      </c>
       <c r="N35" s="4"/>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>32</v>
       </c>
@@ -2356,8 +2950,23 @@
       <c r="F36" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="M36">
+        <v>32</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>33</v>
       </c>
@@ -2373,8 +2982,23 @@
       <c r="F37" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="M37">
+        <v>33</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>34</v>
       </c>
@@ -2390,8 +3014,23 @@
       <c r="F38" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="M38">
+        <v>34</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>35</v>
       </c>
@@ -2407,8 +3046,23 @@
       <c r="F39" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" s="2" customFormat="1">
+      <c r="M39">
+        <v>35</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" s="2" customFormat="1">
       <c r="A40" s="2">
         <v>36</v>
       </c>
@@ -2425,10 +3079,15 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="M40" s="2">
+        <v>36</v>
+      </c>
       <c r="N40" s="4"/>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>37</v>
       </c>
@@ -2444,8 +3103,23 @@
       <c r="F41" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="M41">
+        <v>37</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>38</v>
       </c>
@@ -2461,8 +3135,23 @@
       <c r="F42" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="M42">
+        <v>38</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>39</v>
       </c>
@@ -2478,8 +3167,23 @@
       <c r="F43" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="M43">
+        <v>39</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>40</v>
       </c>
@@ -2495,13 +3199,33 @@
       <c r="F44" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="M44">
+        <v>40</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" s="2" customFormat="1">
+      <c r="M45">
+        <v>41</v>
+      </c>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+    </row>
+    <row r="46" spans="1:17" s="2" customFormat="1">
       <c r="A46" s="2">
         <v>42</v>
       </c>
@@ -2518,12 +3242,16 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="M46" s="2">
+        <v>42</v>
+      </c>
       <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C3:K3"/>
+    <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Avoiding node-23 which has only 4 processors.
</commit_message>
<xml_diff>
--- a/Workflow/dahl nodes.xlsx
+++ b/Workflow/dahl nodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2014-11-29" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="38">
   <si>
     <t>Node</t>
   </si>
@@ -204,8 +204,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="301">
+  <cellStyleXfs count="349">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -523,14 +571,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="301">
+  <cellStyles count="349">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -681,6 +729,30 @@
     <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -831,6 +903,30 @@
     <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1187,17 +1283,17 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
       <c r="P3" t="s">
         <v>6</v>
       </c>
@@ -1981,9 +2077,9 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1460" topLeftCell="A20" activePane="bottomLeft"/>
+      <pane ySplit="1460" topLeftCell="A2" activePane="bottomLeft"/>
       <selection activeCell="L3" sqref="L3"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18:Q18"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2007,27 +2103,27 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
       <c r="L3" s="5"/>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -2057,7 +2153,7 @@
       <c r="K4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -2142,6 +2238,18 @@
       <c r="A11">
         <v>7</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="M11">
         <v>7</v>
       </c>
@@ -2179,13 +2287,13 @@
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M13">
         <v>9</v>
@@ -2199,7 +2307,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
@@ -2250,7 +2358,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
@@ -2271,16 +2379,28 @@
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M17">
         <v>13</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2291,7 +2411,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
@@ -2302,17 +2422,17 @@
       <c r="M18">
         <v>14</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q18" s="6" t="s">
-        <v>12</v>
+      <c r="O18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2323,7 +2443,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
@@ -2341,7 +2461,7 @@
         <v>20</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>28</v>
@@ -2355,13 +2475,13 @@
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M20">
         <v>16</v>
@@ -2373,7 +2493,7 @@
         <v>20</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>28</v>
@@ -2387,7 +2507,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
@@ -2402,10 +2522,10 @@
         <v>6</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>28</v>
@@ -2419,7 +2539,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
@@ -2437,7 +2557,7 @@
         <v>21</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>28</v>
@@ -2450,14 +2570,14 @@
       <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>20</v>
+      <c r="D23" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>15</v>
+      <c r="F23" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="M23">
         <v>19</v>
@@ -2469,7 +2589,7 @@
         <v>21</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>28</v>
@@ -2480,15 +2600,27 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="M24">
@@ -2498,10 +2630,10 @@
         <v>6</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>28</v>
@@ -2515,25 +2647,25 @@
         <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="M25">
         <v>21</v>
@@ -2545,7 +2677,7 @@
         <v>22</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>28</v>
@@ -2559,7 +2691,7 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>25</v>
@@ -2571,7 +2703,7 @@
         <v>26</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>27</v>
@@ -2589,55 +2721,34 @@
         <v>22</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27">
+    <row r="27" spans="1:17" s="2" customFormat="1">
+      <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M27">
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="2">
         <v>23</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:17" s="2" customFormat="1">
       <c r="A28" s="2">

</xml_diff>

<commit_message>
Edits to nodes document.
</commit_message>
<xml_diff>
--- a/Workflow/dahl nodes.xlsx
+++ b/Workflow/dahl nodes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
@@ -121,9 +121,6 @@
     <t>US, UK, JP, AT</t>
   </si>
   <si>
-    <t>R version 2.1</t>
-  </si>
-  <si>
     <t>US, UK, JP</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>US, UK, JP, CN, ZA, SA, IR, TZ, ZM</t>
+  </si>
+  <si>
+    <t>Now available, if needed</t>
   </si>
 </sst>
 </file>
@@ -2077,9 +2077,9 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1460" topLeftCell="A2" activePane="bottomLeft"/>
+      <pane ySplit="1460" topLeftCell="A18" activePane="bottomLeft"/>
       <selection activeCell="L3" sqref="L3"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2429,7 +2429,7 @@
         <v>20</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>28</v>
@@ -2461,7 +2461,7 @@
         <v>20</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>28</v>
@@ -2493,7 +2493,7 @@
         <v>20</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>28</v>
@@ -2525,7 +2525,7 @@
         <v>21</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>28</v>
@@ -2557,7 +2557,7 @@
         <v>21</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>28</v>
@@ -2589,7 +2589,7 @@
         <v>21</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>28</v>
@@ -2633,7 +2633,7 @@
         <v>22</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>28</v>
@@ -2677,7 +2677,7 @@
         <v>22</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>28</v>
@@ -2721,7 +2721,7 @@
         <v>22</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>28</v>
@@ -2813,7 +2813,7 @@
         <v>20</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>19</v>
@@ -2857,7 +2857,7 @@
         <v>20</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>19</v>
@@ -2926,7 +2926,7 @@
         <v>20</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>19</v>
@@ -2970,7 +2970,7 @@
         <v>21</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>19</v>
@@ -3014,7 +3014,7 @@
         <v>21</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>19</v>
@@ -3071,7 +3071,7 @@
         <v>21</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>19</v>
@@ -3103,7 +3103,7 @@
         <v>22</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>19</v>
@@ -3135,7 +3135,7 @@
         <v>22</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>19</v>
@@ -3167,7 +3167,7 @@
         <v>22</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>19</v>
@@ -3178,7 +3178,7 @@
         <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -3224,7 +3224,7 @@
         <v>20</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q41" s="1" t="s">
         <v>15</v>
@@ -3256,7 +3256,7 @@
         <v>21</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>15</v>
@@ -3288,7 +3288,7 @@
         <v>22</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>15</v>
@@ -3320,7 +3320,7 @@
         <v>17</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>12</v>

</xml_diff>